<commit_message>
6.19 Reverse words in a sentence
</commit_message>
<xml_diff>
--- a/List_of_Problems.xlsx
+++ b/List_of_Problems.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
   <si>
     <t>Dutch National Flag</t>
   </si>
@@ -134,6 +134,16 @@
     <t>GFG uses char* naturally similar to mine. 
 EPI uses string class which appears only in C++. StringToInt, IntToString
 GFG uses sprintf convert int to string.</t>
+  </si>
+  <si>
+    <t>Reverse All Words in Sentence</t>
+  </si>
+  <si>
+    <t>I did by not using string class. The Algorithm is similar to EPI
+GFG uses slightly # algo. While  switch step 1 &amp; 2 with me.</t>
+  </si>
+  <si>
+    <t>http://www.geeksforgeeks.org/reverse-words-in-a-given-string/</t>
   </si>
 </sst>
 </file>
@@ -559,10 +569,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -675,7 +685,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="43.2">
+    <row r="9" spans="1:7" ht="51.6" customHeight="1">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -703,7 +713,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" ht="27" customHeight="1">
       <c r="F11" s="1" t="s">
         <v>32</v>
       </c>
@@ -711,7 +721,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="43.2">
+    <row r="12" spans="1:7" ht="52.2" customHeight="1">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -726,6 +736,23 @@
       </c>
       <c r="G12" s="3" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="40.200000000000003" customHeight="1">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13">
+        <v>6.19</v>
+      </c>
+      <c r="E13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -737,9 +764,10 @@
     <hyperlink ref="F10" r:id="rId5"/>
     <hyperlink ref="F11" r:id="rId6"/>
     <hyperlink ref="F12" r:id="rId7"/>
+    <hyperlink ref="F13" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId8"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId9"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
6.21 update some ntes
</commit_message>
<xml_diff>
--- a/List_of_Problems.xlsx
+++ b/List_of_Problems.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Abbre.Web" sheetId="2" r:id="rId1"/>
     <sheet name="Problems" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Note-Overall" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="56">
   <si>
     <t>Dutch National Flag</t>
   </si>
@@ -188,6 +188,15 @@
     <t>GFG is different when removing characters only. This is interesting using State Machine. I will code this when second returns.
 EIP uses string class to resize when adding characters
 My code runs successfully with gcc. VS shows runtime error because write to outboud</t>
+  </si>
+  <si>
+    <t>Might need to code Google question with string with</t>
+  </si>
+  <si>
+    <t>Note string class in C++</t>
+  </si>
+  <si>
+    <t>resize()</t>
   </si>
 </sst>
 </file>
@@ -617,8 +626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="D10" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -874,12 +883,43 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="44.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C1" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
6.22 and 6.23 is a Facebook interview (GFG)
</commit_message>
<xml_diff>
--- a/List_of_Problems.xlsx
+++ b/List_of_Problems.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Abbre.Web" sheetId="2" r:id="rId1"/>
     <sheet name="Problems" sheetId="1" r:id="rId2"/>
     <sheet name="Note-Overall" sheetId="3" r:id="rId3"/>
+    <sheet name="OthersGithub" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="67">
   <si>
     <t>Dutch National Flag</t>
   </si>
@@ -197,6 +198,40 @@
   </si>
   <si>
     <t>resize()</t>
+  </si>
+  <si>
+    <t>https://github.com/jiefenghaspower/codePractise</t>
+  </si>
+  <si>
+    <t>http://www.geeksforgeeks.org/sort-an-array-of-0s-1s-and-2s/</t>
+  </si>
+  <si>
+    <t>If condition is O(n) then we can use counting sort. If condition is only allow one traverse then have to use 3-way parition with high, equal, smaller index</t>
+  </si>
+  <si>
+    <t>http://noteworthyalgorithms.blogspot.com/</t>
+  </si>
+  <si>
+    <t>Regular Expression</t>
+  </si>
+  <si>
+    <t>6.23</t>
+  </si>
+  <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t>6.22</t>
+  </si>
+  <si>
+    <t>EPI good to learn recursive with increase string index</t>
+  </si>
+  <si>
+    <t>http://www.geeksforgeeks.org/forums/topic/facebook-interview-question-for-software-engineerdeveloper-0-2-years-about-algorithms-data-str/</t>
+  </si>
+  <si>
+    <t>EPI hard to understand. 
+I code facebook question interview. GFG does not provide "Official" solution.</t>
   </si>
 </sst>
 </file>
@@ -624,10 +659,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView topLeftCell="D10" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -674,6 +709,12 @@
       <c r="E2" t="s">
         <v>18</v>
       </c>
+      <c r="F2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
@@ -859,6 +900,38 @@
       </c>
       <c r="G17" s="3" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" s="1"/>
+      <c r="G18" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="28.8">
+      <c r="A19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" t="s">
+        <v>50</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -875,9 +948,11 @@
     <hyperlink ref="F15" r:id="rId10"/>
     <hyperlink ref="F16" r:id="rId11"/>
     <hyperlink ref="F17" r:id="rId12"/>
+    <hyperlink ref="F2" r:id="rId13"/>
+    <hyperlink ref="F19" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId13"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId15"/>
 </worksheet>
 </file>
 
@@ -885,7 +960,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -922,4 +997,36 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="42.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
7.2 Checking for cycle in linked list
Also upload Programming Algorithms code
</commit_message>
<xml_diff>
--- a/List_of_Problems.xlsx
+++ b/List_of_Problems.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="80">
   <si>
     <t>Dutch National Flag</t>
   </si>
@@ -247,6 +247,34 @@
     <t>Idea of GFG and EPI is similar. Each loop take out smallest node and then insert into tail of result node. Notice result node is space O(1). (I will code *second returns*)
 CIQ is just recursive ((I will code *second returns*))
 My idea is like brute force. One list is dest and find appropirate position for each element in other list.</t>
+  </si>
+  <si>
+    <t>Checking for Cyclicity</t>
+  </si>
+  <si>
+    <t>7.2</t>
+  </si>
+  <si>
+    <t>4.6 -&gt;4.14</t>
+  </si>
+  <si>
+    <t>x Floyd algthm</t>
+  </si>
+  <si>
+    <t>http://www.geeksforgeeks.org/detect-and-remove-loop-in-a-linked-list/</t>
+  </si>
+  <si>
+    <t>http://www.geeksforgeeks.org/write-a-c-function-to-detect-loop-in-a-linked-list/</t>
+  </si>
+  <si>
+    <t>PP</t>
+  </si>
+  <si>
+    <t>Programming Problems</t>
+  </si>
+  <si>
+    <t>GFG shows 2 methods, kind of similar when count the number of nodes in cycle.
+I wrote code in C++ style with class.</t>
   </si>
 </sst>
 </file>
@@ -618,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -664,6 +692,14 @@
         <v>15</v>
       </c>
     </row>
+    <row r="5" spans="1:3">
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" t="s">
+        <v>78</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1"/>
@@ -674,10 +710,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E14" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H25" sqref="H24:H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -686,12 +723,13 @@
     <col min="2" max="2" width="8.88671875" style="5"/>
     <col min="3" max="3" width="14.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="65.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="68.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="65.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="68.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -705,74 +743,77 @@
         <v>12</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="5">
         <v>6.1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="5">
         <v>6.2</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="5">
         <v>6.3</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
-      <c r="F5" s="1" t="s">
+    <row r="5" spans="1:8">
+      <c r="G5" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="5">
         <v>6.12</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -780,94 +821,94 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="43.2">
+    <row r="8" spans="1:8" ht="43.2">
       <c r="A8" t="s">
         <v>23</v>
       </c>
       <c r="B8" s="5">
         <v>6.13</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="H8" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="51.6" customHeight="1">
+    <row r="9" spans="1:8" ht="51.6" customHeight="1">
       <c r="A9" t="s">
         <v>26</v>
       </c>
       <c r="B9" s="5">
         <v>6.15</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="H9" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="43.2">
+    <row r="10" spans="1:8" ht="43.2">
       <c r="A10" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="27" customHeight="1">
-      <c r="F11" s="1" t="s">
+    <row r="11" spans="1:8" ht="27" customHeight="1">
+      <c r="G11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="52.2" customHeight="1">
+    <row r="12" spans="1:8" ht="52.2" customHeight="1">
       <c r="A12" t="s">
         <v>34</v>
       </c>
       <c r="B12" s="5">
         <v>6.18</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="H12" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="40.200000000000003" customHeight="1">
+    <row r="13" spans="1:8" ht="40.200000000000003" customHeight="1">
       <c r="A13" t="s">
         <v>37</v>
       </c>
       <c r="B13" s="5">
         <v>6.19</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="H13" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="43.2">
+    <row r="14" spans="1:8" ht="43.2">
       <c r="A14" s="3" t="s">
         <v>41</v>
       </c>
@@ -877,79 +918,79 @@
       <c r="C14" t="s">
         <v>42</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="H14" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
-      <c r="F15" s="1" t="s">
+    <row r="15" spans="1:8">
+      <c r="G15" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
-      <c r="F16" s="1" t="s">
+    <row r="16" spans="1:8">
+      <c r="G16" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="72">
+    <row r="17" spans="1:8" ht="72">
       <c r="A17" t="s">
         <v>49</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>50</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="H17" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>61</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>50</v>
       </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="3" t="s">
+      <c r="G18" s="1"/>
+      <c r="H18" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="28.8">
+    <row r="19" spans="1:8" ht="28.8">
       <c r="A19" t="s">
         <v>59</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>50</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="H19" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="86.4">
+    <row r="20" spans="1:8" ht="86.4">
       <c r="A20" s="3" t="s">
         <v>66</v>
       </c>
@@ -959,36 +1000,66 @@
       <c r="C20">
         <v>4.28</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>50</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="H20" s="3" t="s">
         <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="28.8">
+      <c r="A21" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21">
+        <v>2.23</v>
+      </c>
+      <c r="F21" t="s">
+        <v>74</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="G22" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F4" r:id="rId1"/>
-    <hyperlink ref="F5" r:id="rId2"/>
-    <hyperlink ref="F8" r:id="rId3"/>
-    <hyperlink ref="F9" r:id="rId4"/>
-    <hyperlink ref="F10" r:id="rId5"/>
-    <hyperlink ref="F11" r:id="rId6"/>
-    <hyperlink ref="F12" r:id="rId7"/>
-    <hyperlink ref="F13" r:id="rId8"/>
-    <hyperlink ref="F14" r:id="rId9"/>
-    <hyperlink ref="F15" r:id="rId10"/>
-    <hyperlink ref="F16" r:id="rId11"/>
-    <hyperlink ref="F17" r:id="rId12"/>
-    <hyperlink ref="F2" r:id="rId13"/>
-    <hyperlink ref="F19" r:id="rId14"/>
-    <hyperlink ref="F20" r:id="rId15"/>
+    <hyperlink ref="G4" r:id="rId1"/>
+    <hyperlink ref="G5" r:id="rId2"/>
+    <hyperlink ref="G8" r:id="rId3"/>
+    <hyperlink ref="G9" r:id="rId4"/>
+    <hyperlink ref="G10" r:id="rId5"/>
+    <hyperlink ref="G11" r:id="rId6"/>
+    <hyperlink ref="G12" r:id="rId7"/>
+    <hyperlink ref="G13" r:id="rId8"/>
+    <hyperlink ref="G14" r:id="rId9"/>
+    <hyperlink ref="G15" r:id="rId10"/>
+    <hyperlink ref="G16" r:id="rId11"/>
+    <hyperlink ref="G17" r:id="rId12"/>
+    <hyperlink ref="G2" r:id="rId13"/>
+    <hyperlink ref="G19" r:id="rId14"/>
+    <hyperlink ref="G20" r:id="rId15"/>
+    <hyperlink ref="G21" r:id="rId16"/>
+    <hyperlink ref="G22" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId16"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId18"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
7.6 odd even list
</commit_message>
<xml_diff>
--- a/List_of_Problems.xlsx
+++ b/List_of_Problems.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="94">
   <si>
     <t>Dutch National Flag</t>
   </si>
@@ -249,9 +249,6 @@
 My idea is like brute force. One list is dest and find appropirate position for each element in other list.</t>
   </si>
   <si>
-    <t>Checking for Cyclicity</t>
-  </si>
-  <si>
     <t>7.2</t>
   </si>
   <si>
@@ -275,6 +272,56 @@
   <si>
     <t>GFG shows 2 methods, kind of similar when count the number of nodes in cycle.
 I wrote code in C++ style with class.</t>
+  </si>
+  <si>
+    <t>Checking for 
+Cyclicity</t>
+  </si>
+  <si>
+    <t>Median of sorted
+circual linked list</t>
+  </si>
+  <si>
+    <t>7.3</t>
+  </si>
+  <si>
+    <t>Find minimum first. Notice when every elments are equal</t>
+  </si>
+  <si>
+    <t>Overlapping List
+No Cycle</t>
+  </si>
+  <si>
+    <t>7.4</t>
+  </si>
+  <si>
+    <t>4.17 -&gt; 4.23</t>
+  </si>
+  <si>
+    <t>CIQ has stack idea is good. Others shows the same idea when find different length between lists</t>
+  </si>
+  <si>
+    <t>Overlapping List
+with Cycle</t>
+  </si>
+  <si>
+    <t>7.5</t>
+  </si>
+  <si>
+    <t>Check cycle. If cycle then check cycle overlap. Then use Foyd algorithm</t>
+  </si>
+  <si>
+    <t>Even Odd Merge</t>
+  </si>
+  <si>
+    <t>7.6</t>
+  </si>
+  <si>
+    <t>EPI is similar to my code. 
+GFG is different requirement but good to learn move odd nodes to the end of list first technique</t>
+  </si>
+  <si>
+    <t>http://www.geeksforgeeks.org/segregate-even-and-odd-elements-in-a-linked-list/</t>
   </si>
 </sst>
 </file>
@@ -694,10 +741,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="B5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" t="s">
         <v>77</v>
-      </c>
-      <c r="C5" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -710,11 +757,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H25" sqref="H24:H25"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -743,7 +790,7 @@
         <v>12</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>3</v>
@@ -1011,31 +1058,84 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="28.8">
-      <c r="A21" t="s">
+      <c r="A21" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="C21" t="s">
         <v>72</v>
-      </c>
-      <c r="C21" t="s">
-        <v>73</v>
       </c>
       <c r="E21">
         <v>2.23</v>
       </c>
       <c r="F21" t="s">
+        <v>73</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="G21" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="H21" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="G22" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="28.8">
+      <c r="A23" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="28.8">
+      <c r="A24" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" t="s">
+        <v>85</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="28.8">
+      <c r="A25" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="43.2">
+      <c r="A26" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F26" t="s">
+        <v>50</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1057,9 +1157,10 @@
     <hyperlink ref="G20" r:id="rId15"/>
     <hyperlink ref="G21" r:id="rId16"/>
     <hyperlink ref="G22" r:id="rId17"/>
+    <hyperlink ref="G26" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId18"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId19"/>
 </worksheet>
 </file>
 

</xml_diff>